<commit_message>
Stratified both studies by subj id + added # of subjects to mean/sd
</commit_message>
<xml_diff>
--- a/PCD_mean_sd_trembling_rambling.xlsx
+++ b/PCD_mean_sd_trembling_rambling.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+  <si>
+    <t>Cohort</t>
+  </si>
   <si>
     <t>Component</t>
   </si>
@@ -26,6 +29,15 @@
   </si>
   <si>
     <t>Standard_Deviation</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
+    <t>100s</t>
+  </si>
+  <si>
+    <t>200s</t>
   </si>
   <si>
     <t>Rambling</t>
@@ -395,13 +407,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,61 +426,171 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>-0.03658395628494156</v>
+      </c>
+      <c r="E2">
+        <v>0.3931959601114328</v>
+      </c>
+      <c r="F2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>0.03244129903099933</v>
-      </c>
-      <c r="D2">
-        <v>0.4344078916579623</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>-0.08625170631061047</v>
+      </c>
+      <c r="E3">
+        <v>1.945771240426168</v>
+      </c>
+      <c r="F3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>-8.454678618618019E-07</v>
+      </c>
+      <c r="E4">
+        <v>4.245181673844462E-05</v>
+      </c>
+      <c r="F4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>2.000999336161684E-05</v>
+      </c>
+      <c r="E5">
+        <v>0.000452942851766289</v>
+      </c>
+      <c r="F5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>0.01482594629788548</v>
-      </c>
-      <c r="D3">
-        <v>1.897018025969729</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>-8.118655340845376E-07</v>
-      </c>
-      <c r="D4">
-        <v>4.294336950437045E-05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>0.09327416293317954</v>
+      </c>
+      <c r="E6">
+        <v>0.4596924592754691</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>-6.829874690630534E-06</v>
-      </c>
-      <c r="D5">
-        <v>0.0006123459011225655</v>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>0.1039070088240599</v>
+      </c>
+      <c r="E7">
+        <v>1.850877978605084</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>-7.822513613717468E-07</v>
+      </c>
+      <c r="E8">
+        <v>4.342558459508203E-05</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>-3.048420284778794E-05</v>
+      </c>
+      <c r="E9">
+        <v>0.0007241024510988817</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code works off of IEP and IEP residuals rather than just high freq/low freq filtered residuals
</commit_message>
<xml_diff>
--- a/PCD_mean_sd_trembling_rambling.xlsx
+++ b/PCD_mean_sd_trembling_rambling.xlsx
@@ -444,10 +444,10 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>-0.03610924974098829</v>
+        <v>-0.03644326811879168</v>
       </c>
       <c r="E2">
-        <v>0.3934390525010951</v>
+        <v>0.393865553482251</v>
       </c>
       <c r="F2">
         <v>18</v>
@@ -464,10 +464,10 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>-0.068491860178233</v>
+        <v>0.2808990339019236</v>
       </c>
       <c r="E3">
-        <v>1.968250759181248</v>
+        <v>6.57676811390915</v>
       </c>
       <c r="F3">
         <v>18</v>
@@ -484,10 +484,10 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>-0.0004755520118151302</v>
+        <v>-0.0001415336340117438</v>
       </c>
       <c r="E4">
-        <v>0.008809332796839315</v>
+        <v>0.01083971667409135</v>
       </c>
       <c r="F4">
         <v>18</v>
@@ -504,10 +504,10 @@
         <v>11</v>
       </c>
       <c r="D5">
-        <v>-0.01773983613901586</v>
+        <v>-0.3671307302191725</v>
       </c>
       <c r="E5">
-        <v>0.1425085021433249</v>
+        <v>6.128582539354844</v>
       </c>
       <c r="F5">
         <v>18</v>
@@ -524,10 +524,10 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <v>0.09355037708151873</v>
+        <v>0.09342891388835872</v>
       </c>
       <c r="E6">
-        <v>0.4593153229327364</v>
+        <v>0.4583074153935279</v>
       </c>
       <c r="F6">
         <v>20</v>
@@ -544,10 +544,10 @@
         <v>11</v>
       </c>
       <c r="D7">
-        <v>0.1110863969870958</v>
+        <v>0.5989335063986924</v>
       </c>
       <c r="E7">
-        <v>1.857472495525724</v>
+        <v>6.630267284365771</v>
       </c>
       <c r="F7">
         <v>20</v>
@@ -564,10 +564,10 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <v>-0.000276996399700548</v>
+        <v>-0.0001555332065405596</v>
       </c>
       <c r="E8">
-        <v>0.01173474158995077</v>
+        <v>0.007012150680553096</v>
       </c>
       <c r="F8">
         <v>20</v>
@@ -584,10 +584,10 @@
         <v>11</v>
       </c>
       <c r="D9">
-        <v>-0.007209872365883598</v>
+        <v>-0.4950569817774801</v>
       </c>
       <c r="E9">
-        <v>0.15378831633937</v>
+        <v>6.199878703985113</v>
       </c>
       <c r="F9">
         <v>20</v>

</xml_diff>